<commit_message>
inclui metodologia da receita
</commit_message>
<xml_diff>
--- a/metod-receita.xlsx
+++ b/metod-receita.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiago/Documents/GitHub/orcamento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274C80D4-5CC9-F243-8CE7-B50D26E15D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2D9794-2F76-884A-BBF5-6A17A2A7AAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="21600" xr2:uid="{46DE55F4-85F8-EB43-81D4-3CEA551AD2E3}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16780" xr2:uid="{46DE55F4-85F8-EB43-81D4-3CEA551AD2E3}"/>
   </bookViews>
   <sheets>
     <sheet name="metod-receita" sheetId="1" r:id="rId1"/>
@@ -884,46 +884,118 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="37" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1303,718 +1375,722 @@
   <dimension ref="B2:M43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="B2" sqref="B2:H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.1640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="2.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="36" customWidth="1"/>
+    <col min="6" max="6" width="3.1640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="2:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="16" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B3" s="2">
+    <row r="3" spans="2:13" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="9">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="19">
         <v>1</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="25" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="21">
+    <row r="4" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="8"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="19">
         <v>2</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="2">
+      <c r="H4" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="B5" s="8"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="6"/>
-      <c r="F6" s="22">
+    <row r="6" spans="2:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="B6" s="8"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="11"/>
+      <c r="F6" s="20">
         <v>14</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="28" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="23">
+    <row r="7" spans="2:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="B7" s="8"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="21">
         <v>2</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="2">
+    <row r="8" spans="2:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="B8" s="8"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="9">
         <v>3</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="22">
         <v>1</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="24">
+      <c r="H8" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="B9" s="8"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="22">
         <v>2</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="24">
+    <row r="10" spans="2:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="B10" s="11"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="22">
         <v>3</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="24">
+      <c r="H10" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="2:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="B11" s="11"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="22">
         <v>4</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="24">
+    <row r="12" spans="2:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="B12" s="11"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="22">
         <v>5</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="24">
+      <c r="H12" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="11"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="22">
         <v>6</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="24">
+      <c r="H13" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="B14" s="11"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="22">
         <v>9</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8">
+      <c r="H14" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="B15" s="11"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="12">
         <v>4</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="22">
         <v>1</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8">
+      <c r="H15" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="B16" s="11"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="12">
         <v>5</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="24">
+      <c r="F16" s="22">
         <v>1</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="6">
+      <c r="H16" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B17" s="11"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="11">
         <v>6</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="24">
+      <c r="F17" s="22">
         <v>1</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="24">
+      <c r="H17" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B18" s="11"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="22">
         <v>2</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="24">
+      <c r="H18" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B19" s="11"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="22">
         <v>3</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="24">
+      <c r="H19" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B20" s="11"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="22">
         <v>4</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="24">
+    <row r="21" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B21" s="11"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="22">
         <v>9</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H21" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="2">
+      <c r="H21" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="11"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="9">
         <v>7</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="24">
+      <c r="F22" s="22">
         <v>2</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H22" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="24">
+      <c r="H22" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B23" s="11"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="22">
         <v>3</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="24">
+      <c r="H23" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B24" s="11"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="22">
         <v>4</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="24">
+      <c r="H24" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B25" s="11"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="22">
         <v>6</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="24">
+      <c r="H25" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B26" s="11"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="22">
         <v>9</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G26" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="2">
+      <c r="H26" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B27" s="11"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="9">
         <v>9</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="24">
+      <c r="F27" s="22">
         <v>1</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H27" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="24">
+      <c r="H27" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="B28" s="11"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="22">
         <v>2</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="24">
+      <c r="H28" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="B29" s="11"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="22">
         <v>3</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="G29" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H29" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="24">
+      <c r="H29" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B30" s="11"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="22">
         <v>4</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="G30" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H30" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="4"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="24">
+      <c r="H30" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B31" s="10"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="22">
         <v>9</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G31" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="H31" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="2">
+      <c r="H31" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B32" s="9">
         <v>2</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="9">
         <v>1</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="21">
+      <c r="F32" s="19">
         <v>1</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="H32" s="31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="23">
+    <row r="33" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B33" s="11"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="21">
         <v>2</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G33" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="H33" s="31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" s="6"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="2">
+    <row r="34" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B34" s="11"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="9">
         <v>2</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="21">
+      <c r="F34" s="19">
         <v>1</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B35" s="6"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="23">
+      <c r="H34" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B35" s="11"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="21">
         <v>2</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="G35" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H35" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B36" s="6"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="6">
+      <c r="H35" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B36" s="11"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="11">
         <v>3</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="F36" s="22">
+      <c r="F36" s="20">
         <v>1</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="G36" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H36" s="18" t="s">
+      <c r="H36" s="29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="2">
+    <row r="37" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B37" s="11"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="9">
         <v>4</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="F37" s="21">
+      <c r="F37" s="19">
         <v>2</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H37" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="6"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="22">
+      <c r="H37" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B38" s="11"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="20">
         <v>3</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="G38" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="H38" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="6"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="22">
+      <c r="H38" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B39" s="11"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="20">
         <v>4</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="G39" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="H39" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="6"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="22">
+      <c r="H39" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B40" s="11"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="20">
         <v>6</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="G40" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H40" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B41" s="6"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="23">
+      <c r="H40" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B41" s="11"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="21">
         <v>9</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="G41" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="H41" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="6"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="2">
+      <c r="H41" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B42" s="11"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="9">
         <v>9</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="F42" s="21">
+      <c r="F42" s="19">
         <v>2</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G42" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H42" s="13" t="s">
+      <c r="H42" s="32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B43" s="4"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="23">
+    <row r="43" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="B43" s="10"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="21">
         <v>3</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="G43" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="H43" s="13" t="s">
+      <c r="H43" s="32" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="E22:E26"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:C17"/>
+    <mergeCell ref="B3:B9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>